<commit_message>
not dure what changed
</commit_message>
<xml_diff>
--- a/EmployeeSQL/ERD Research.xlsx
+++ b/EmployeeSQL/ERD Research.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="8_{0082C1A3-AC08-4FB0-A02C-3FDFB6294389}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{20DC1231-1F0B-4A24-8D3F-B07FDADA1D6F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2625" windowWidth="25440" windowHeight="15390" xr2:uid="{626BB903-EB61-4B30-A8C1-C1A43630F9AB}"/>
+    <workbookView xWindow="-18885" yWindow="-105" windowWidth="17280" windowHeight="8970" xr2:uid="{626BB903-EB61-4B30-A8C1-C1A43630F9AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
   <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>